<commit_message>
moved date for Lab00 to 2-2-24
</commit_message>
<xml_diff>
--- a/CS320-Spring2024Calendar(1-26-24).xlsx
+++ b/CS320-Spring2024Calendar(1-26-24).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\donha\cs320-spring2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00C25C41-400D-4566-969F-629C5C55FFD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3882A686-D6A5-497C-B59A-B0F066E8395C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2415" yWindow="338" windowWidth="22417" windowHeight="14857" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5490" yWindow="0" windowWidth="22433" windowHeight="14857" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Calendar-Sp24" sheetId="1" r:id="rId1"/>
@@ -131,25 +131,6 @@
     <t>Final Presentation &amp; Demo</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Lecture 12: Version Control
-(Git)
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Git Lab: Part I
-(assigned)</t>
-    </r>
-  </si>
-  <si>
     <t>Web
 Applications II
 Web Applications Labs Review</t>
@@ -470,9 +451,15 @@
     <t>Team Project Assignment</t>
   </si>
   <si>
+    <t>Prep Exam
+due Mon, 1-29-24 before class
+-------&gt;
+(Marmoset)</t>
+  </si>
+  <si>
     <r>
-      <t xml:space="preserve">Lecture 2:
-HTML &amp; CSS, ChatGPT, and self-learning
+      <t xml:space="preserve">Lecture 0: Course Overview
+Guest: Dan Palmieri
 </t>
     </r>
     <r>
@@ -484,41 +471,19 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Lab 1: HTML/CSS Resume
- (assigned)</t>
+      <t>Prep Exam
+(assigned)</t>
     </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Lab 0: ChatGPT
-due before class
-(Marmoset)</t>
-    </r>
+  </si>
+  <si>
+    <t>CS320: SW Engineering - Spring 2024 Schedule
+(as of 1-30-2024, subject to change)</t>
   </si>
   <si>
     <r>
       <t xml:space="preserve">Lecture 0:
 SW Enginering Intro 
 Calendar, Projects
-Lecture 1: OOP &amp; ChatGPT
 </t>
     </r>
     <r>
@@ -548,15 +513,10 @@
     </r>
   </si>
   <si>
-    <t>Prep Exam
-due Mon, 1-29-24 before class
--------&gt;
-(Marmoset)</t>
-  </si>
-  <si>
     <r>
-      <t xml:space="preserve">Lecture 0: Course Overview
-Guest: Dan Palmieri
+      <t xml:space="preserve">Lecture 1: OOP &amp; ChatGPT
+Lecture 2:
+HTML &amp; CSS, ChatGPT, and self-learning
 </t>
     </r>
     <r>
@@ -568,13 +528,54 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Prep Exam
+      <t>Lab 1: HTML/CSS Resume
+ (assigned)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Project Introductions
+Lecture 12: Version Control
+(Git)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Git Lab: Part I
 (assigned)</t>
     </r>
-  </si>
-  <si>
-    <t>CS320: SW Engineering - Spring 2024 Schedule
-(as of 1-26-2024, subject to change)</t>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Lab 0: ChatGPT
+due 7:00am
+(Marmoset)</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1671,74 +1672,74 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2050,7 +2051,7 @@
   <dimension ref="A1:R42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection sqref="A1:I1"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2072,17 +2073,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="53.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="132" t="s">
-        <v>77</v>
-      </c>
-      <c r="B1" s="133"/>
-      <c r="C1" s="133"/>
-      <c r="D1" s="133"/>
-      <c r="E1" s="133"/>
-      <c r="F1" s="133"/>
-      <c r="G1" s="133"/>
-      <c r="H1" s="133"/>
-      <c r="I1" s="134"/>
+      <c r="A1" s="149" t="s">
+        <v>74</v>
+      </c>
+      <c r="B1" s="150"/>
+      <c r="C1" s="150"/>
+      <c r="D1" s="150"/>
+      <c r="E1" s="150"/>
+      <c r="F1" s="150"/>
+      <c r="G1" s="150"/>
+      <c r="H1" s="150"/>
+      <c r="I1" s="151"/>
     </row>
     <row r="2" spans="1:18" s="2" customFormat="1" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A2" s="1" t="s">
@@ -2112,10 +2113,10 @@
       </c>
     </row>
     <row r="3" spans="1:18" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="137">
+      <c r="A3" s="141">
         <v>15</v>
       </c>
-      <c r="B3" s="146" t="s">
+      <c r="B3" s="136" t="s">
         <v>10</v>
       </c>
       <c r="C3" s="67">
@@ -2147,8 +2148,8 @@
       </c>
     </row>
     <row r="4" spans="1:18" ht="75.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A4" s="136"/>
-      <c r="B4" s="147"/>
+      <c r="A4" s="145"/>
+      <c r="B4" s="153"/>
       <c r="C4" s="69" t="s">
         <v>7</v>
       </c>
@@ -2169,17 +2170,17 @@
       </c>
       <c r="G4" s="37"/>
       <c r="H4" s="36" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="I4" s="40"/>
     </row>
     <row r="5" spans="1:18" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="136">
+      <c r="A5" s="145">
         <f>A3 - 1</f>
         <v>14</v>
       </c>
-      <c r="B5" s="141" t="s">
-        <v>34</v>
+      <c r="B5" s="138" t="s">
+        <v>33</v>
       </c>
       <c r="C5" s="7">
         <f>I3 + 1</f>
@@ -2210,30 +2211,30 @@
       </c>
     </row>
     <row r="6" spans="1:18" ht="146.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A6" s="138"/>
-      <c r="B6" s="142"/>
+      <c r="A6" s="142"/>
+      <c r="B6" s="137"/>
       <c r="C6" s="123" t="s">
+        <v>72</v>
+      </c>
+      <c r="D6" s="132" t="s">
         <v>75</v>
-      </c>
-      <c r="D6" s="154" t="s">
-        <v>74</v>
       </c>
       <c r="E6" s="57"/>
       <c r="F6" s="124" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="G6" s="48"/>
-      <c r="H6" s="12" t="s">
-        <v>29</v>
+      <c r="H6" s="47" t="s">
+        <v>77</v>
       </c>
       <c r="I6" s="107"/>
     </row>
     <row r="7" spans="1:18" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A7" s="139">
+      <c r="A7" s="146">
         <f>A5 - 1</f>
         <v>13</v>
       </c>
-      <c r="B7" s="143" t="s">
+      <c r="B7" s="133" t="s">
         <v>11</v>
       </c>
       <c r="C7" s="38">
@@ -2266,32 +2267,32 @@
       </c>
     </row>
     <row r="8" spans="1:18" ht="87.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A8" s="140"/>
-      <c r="B8" s="144"/>
+      <c r="A8" s="139"/>
+      <c r="B8" s="135"/>
       <c r="C8" s="30" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D8" s="47" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E8" s="10"/>
       <c r="F8" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G8" s="27"/>
       <c r="H8" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I8" s="108" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A9" s="140">
+      <c r="A9" s="139">
         <f>A7 - 1</f>
         <v>12</v>
       </c>
-      <c r="B9" s="144"/>
+      <c r="B9" s="135"/>
       <c r="C9" s="14">
         <f>I7 + 1</f>
         <v>11</v>
@@ -2329,13 +2330,13 @@
       <c r="R9" s="117"/>
     </row>
     <row r="10" spans="1:18" ht="80.650000000000006" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="140"/>
-      <c r="B10" s="144"/>
+      <c r="A10" s="139"/>
+      <c r="B10" s="135"/>
       <c r="C10" s="109" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E10" s="11"/>
       <c r="F10" s="10" t="s">
@@ -2343,7 +2344,7 @@
       </c>
       <c r="G10" s="11"/>
       <c r="H10" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I10" s="13"/>
       <c r="L10" s="25"/>
@@ -2355,11 +2356,11 @@
       <c r="R10" s="118"/>
     </row>
     <row r="11" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="140">
+      <c r="A11" s="139">
         <f>A9 -1</f>
         <v>11</v>
       </c>
-      <c r="B11" s="144"/>
+      <c r="B11" s="135"/>
       <c r="C11" s="17">
         <f>I9 + 1</f>
         <v>18</v>
@@ -2397,21 +2398,21 @@
       <c r="R11" s="117"/>
     </row>
     <row r="12" spans="1:18" ht="90.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A12" s="140"/>
-      <c r="B12" s="144"/>
+      <c r="A12" s="139"/>
+      <c r="B12" s="135"/>
       <c r="C12" s="126"/>
       <c r="D12" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E12" s="125" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F12" s="44" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G12" s="42"/>
       <c r="H12" s="49" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I12" s="78"/>
       <c r="L12" s="25"/>
@@ -2423,12 +2424,12 @@
       <c r="R12" s="118"/>
     </row>
     <row r="13" spans="1:18" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A13" s="140">
+      <c r="A13" s="139">
         <f xml:space="preserve"> A11 - 1</f>
         <v>10</v>
       </c>
-      <c r="B13" s="148" t="s">
-        <v>35</v>
+      <c r="B13" s="154" t="s">
+        <v>34</v>
       </c>
       <c r="C13" s="17">
         <f>I11 + 1</f>
@@ -2466,24 +2467,24 @@
       <c r="R13" s="119"/>
     </row>
     <row r="14" spans="1:18" ht="108.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A14" s="145"/>
-      <c r="B14" s="149"/>
+      <c r="A14" s="140"/>
+      <c r="B14" s="134"/>
       <c r="C14" s="29"/>
       <c r="D14" s="128" t="s">
         <v>25</v>
       </c>
       <c r="E14" s="90"/>
       <c r="F14" s="43" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G14" s="89" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H14" s="84" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I14" s="85" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L14" s="119"/>
       <c r="M14" s="25"/>
@@ -2494,11 +2495,11 @@
       <c r="R14" s="119"/>
     </row>
     <row r="15" spans="1:18" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A15" s="137">
+      <c r="A15" s="141">
         <f>A13 - 1</f>
         <v>9</v>
       </c>
-      <c r="B15" s="141" t="s">
+      <c r="B15" s="138" t="s">
         <v>12</v>
       </c>
       <c r="C15" s="67">
@@ -2531,23 +2532,23 @@
       </c>
     </row>
     <row r="16" spans="1:18" ht="93.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A16" s="138"/>
-      <c r="B16" s="142"/>
+      <c r="A16" s="142"/>
+      <c r="B16" s="137"/>
       <c r="C16" s="86" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E16" s="64" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G16" s="93"/>
       <c r="H16" s="64" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I16" s="94"/>
     </row>
@@ -2571,19 +2572,19 @@
         <v>16</v>
       </c>
       <c r="E19" s="31" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F19" s="32" t="s">
         <v>17</v>
       </c>
       <c r="G19" s="131" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H19" s="33" t="s">
         <v>18</v>
       </c>
       <c r="I19" s="63" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:18" s="122" customFormat="1" ht="21.4" thickTop="1" x14ac:dyDescent="0.45">
@@ -2609,19 +2610,19 @@
       <c r="I21" s="119"/>
     </row>
     <row r="22" spans="1:18" ht="54" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A22" s="132" t="str">
+      <c r="A22" s="149" t="str">
         <f>A1</f>
         <v>CS320: SW Engineering - Spring 2024 Schedule
-(as of 1-26-2024, subject to change)</v>
-      </c>
-      <c r="B22" s="133"/>
-      <c r="C22" s="133"/>
-      <c r="D22" s="133"/>
-      <c r="E22" s="133"/>
-      <c r="F22" s="133"/>
-      <c r="G22" s="133"/>
-      <c r="H22" s="133"/>
-      <c r="I22" s="134"/>
+(as of 1-30-2024, subject to change)</v>
+      </c>
+      <c r="B22" s="150"/>
+      <c r="C22" s="150"/>
+      <c r="D22" s="150"/>
+      <c r="E22" s="150"/>
+      <c r="F22" s="150"/>
+      <c r="G22" s="150"/>
+      <c r="H22" s="150"/>
+      <c r="I22" s="151"/>
     </row>
     <row r="23" spans="1:18" s="2" customFormat="1" ht="17.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A23" s="1" t="str">
@@ -2659,11 +2660,11 @@
       </c>
     </row>
     <row r="24" spans="1:18" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A24" s="135">
+      <c r="A24" s="152">
         <f>A15-1</f>
         <v>8</v>
       </c>
-      <c r="B24" s="141" t="s">
+      <c r="B24" s="138" t="s">
         <v>12</v>
       </c>
       <c r="C24" s="95">
@@ -2703,15 +2704,15 @@
       <c r="R24" s="117"/>
     </row>
     <row r="25" spans="1:18" ht="102.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A25" s="136"/>
-      <c r="B25" s="141"/>
+      <c r="A25" s="145"/>
+      <c r="B25" s="138"/>
       <c r="C25" s="51"/>
       <c r="D25" s="22" t="s">
         <v>14</v>
       </c>
       <c r="E25" s="6"/>
       <c r="F25" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G25" s="6"/>
       <c r="H25" s="6" t="s">
@@ -2727,11 +2728,11 @@
       <c r="R25" s="25"/>
     </row>
     <row r="26" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A26" s="136">
+      <c r="A26" s="145">
         <f>A24 - 1</f>
         <v>7</v>
       </c>
-      <c r="B26" s="141"/>
+      <c r="B26" s="138"/>
       <c r="C26" s="7">
         <f>I24 + 1</f>
         <v>17</v>
@@ -2769,26 +2770,26 @@
       <c r="R26" s="117"/>
     </row>
     <row r="27" spans="1:18" ht="129.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A27" s="136"/>
-      <c r="B27" s="141"/>
+      <c r="A27" s="145"/>
+      <c r="B27" s="138"/>
       <c r="C27" s="116"/>
       <c r="D27" s="26" t="s">
         <v>26</v>
       </c>
       <c r="E27" s="129" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F27" s="55" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G27" s="110" t="s">
+        <v>48</v>
+      </c>
+      <c r="H27" s="36" t="s">
+        <v>67</v>
+      </c>
+      <c r="I27" s="115" t="s">
         <v>49</v>
-      </c>
-      <c r="H27" s="36" t="s">
-        <v>68</v>
-      </c>
-      <c r="I27" s="115" t="s">
-        <v>50</v>
       </c>
       <c r="L27" s="25"/>
       <c r="M27" s="117"/>
@@ -2799,11 +2800,11 @@
       <c r="R27" s="25"/>
     </row>
     <row r="28" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A28" s="136">
+      <c r="A28" s="145">
         <f>A26 - 1</f>
         <v>6</v>
       </c>
-      <c r="B28" s="141"/>
+      <c r="B28" s="138"/>
       <c r="C28" s="7">
         <f>I26 + 1</f>
         <v>24</v>
@@ -2841,24 +2842,24 @@
       <c r="R28" s="117"/>
     </row>
     <row r="29" spans="1:18" ht="68.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A29" s="138"/>
-      <c r="B29" s="142"/>
+      <c r="A29" s="142"/>
+      <c r="B29" s="137"/>
       <c r="C29" s="111"/>
       <c r="D29" s="23" t="s">
         <v>22</v>
       </c>
       <c r="E29" s="50" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F29" s="9" t="s">
         <v>23</v>
       </c>
       <c r="G29" s="96"/>
       <c r="H29" s="72" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I29" s="114" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="L29" s="25"/>
       <c r="M29" s="117"/>
@@ -2869,12 +2870,12 @@
       <c r="R29" s="25"/>
     </row>
     <row r="30" spans="1:18" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A30" s="139">
+      <c r="A30" s="146">
         <f>A28 -1</f>
         <v>5</v>
       </c>
-      <c r="B30" s="143" t="s">
-        <v>42</v>
+      <c r="B30" s="133" t="s">
+        <v>41</v>
       </c>
       <c r="C30" s="102">
         <f>I28 + 1</f>
@@ -2905,32 +2906,32 @@
       </c>
     </row>
     <row r="31" spans="1:18" ht="55.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A31" s="150"/>
-      <c r="B31" s="149"/>
+      <c r="A31" s="147"/>
+      <c r="B31" s="134"/>
       <c r="C31" s="127" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D31" s="104" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E31" s="50" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F31" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G31" s="79"/>
       <c r="H31" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I31" s="28"/>
     </row>
     <row r="32" spans="1:18" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A32" s="151">
+      <c r="A32" s="148">
         <f>A30 -1</f>
         <v>4</v>
       </c>
-      <c r="B32" s="143" t="s">
+      <c r="B32" s="133" t="s">
         <v>13</v>
       </c>
       <c r="C32" s="60">
@@ -2963,30 +2964,30 @@
       </c>
     </row>
     <row r="33" spans="1:9" ht="93" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A33" s="140"/>
-      <c r="B33" s="144"/>
+      <c r="A33" s="139"/>
+      <c r="B33" s="135"/>
       <c r="C33" s="29"/>
       <c r="D33" s="112" t="s">
         <v>27</v>
       </c>
       <c r="E33" s="113" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F33" s="12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G33" s="27"/>
       <c r="H33" s="106" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I33" s="28"/>
     </row>
     <row r="34" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A34" s="140">
+      <c r="A34" s="139">
         <f>A32 -1</f>
         <v>3</v>
       </c>
-      <c r="B34" s="144"/>
+      <c r="B34" s="135"/>
       <c r="C34" s="27">
         <f>I32 + 1</f>
         <v>14</v>
@@ -3017,8 +3018,8 @@
       </c>
     </row>
     <row r="35" spans="1:9" ht="38.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A35" s="140"/>
-      <c r="B35" s="144"/>
+      <c r="A35" s="139"/>
+      <c r="B35" s="135"/>
       <c r="C35" s="29"/>
       <c r="D35" s="105" t="s">
         <v>6</v>
@@ -3034,11 +3035,11 @@
       <c r="I35" s="28"/>
     </row>
     <row r="36" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A36" s="140">
+      <c r="A36" s="139">
         <f>A34 -1</f>
         <v>2</v>
       </c>
-      <c r="B36" s="144"/>
+      <c r="B36" s="135"/>
       <c r="C36" s="29">
         <f>I34 + 1</f>
         <v>21</v>
@@ -3069,8 +3070,8 @@
       </c>
     </row>
     <row r="37" spans="1:9" ht="64.150000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A37" s="145"/>
-      <c r="B37" s="149"/>
+      <c r="A37" s="140"/>
+      <c r="B37" s="134"/>
       <c r="C37" s="58"/>
       <c r="D37" s="43" t="s">
         <v>24</v>
@@ -3086,12 +3087,12 @@
       <c r="I37" s="41"/>
     </row>
     <row r="38" spans="1:9" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A38" s="137">
+      <c r="A38" s="141">
         <f>A36 -1</f>
         <v>1</v>
       </c>
-      <c r="B38" s="146" t="s">
-        <v>43</v>
+      <c r="B38" s="136" t="s">
+        <v>42</v>
       </c>
       <c r="C38" s="17">
         <f>I36 + 1</f>
@@ -3122,8 +3123,8 @@
       </c>
     </row>
     <row r="39" spans="1:9" ht="58.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A39" s="138"/>
-      <c r="B39" s="142"/>
+      <c r="A39" s="142"/>
+      <c r="B39" s="137"/>
       <c r="C39" s="99"/>
       <c r="D39" s="49" t="s">
         <v>6</v>
@@ -3134,17 +3135,17 @@
       </c>
       <c r="G39" s="6"/>
       <c r="H39" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I39" s="130" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="40" spans="1:9" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A40" s="152" t="s">
+      <c r="A40" s="143" t="s">
         <v>28</v>
       </c>
-      <c r="B40" s="141" t="s">
+      <c r="B40" s="138" t="s">
         <v>5</v>
       </c>
       <c r="C40" s="20">
@@ -3177,17 +3178,17 @@
       </c>
     </row>
     <row r="41" spans="1:9" ht="134.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A41" s="153"/>
-      <c r="B41" s="142"/>
+      <c r="A41" s="144"/>
+      <c r="B41" s="137"/>
       <c r="C41" s="61" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D41" s="23" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E41" s="62"/>
       <c r="F41" s="23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G41" s="21"/>
       <c r="H41" s="76"/>
@@ -3196,18 +3197,6 @@
     <row r="42" spans="1:9" ht="14.65" thickTop="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="B32:B37"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="B40:B41"/>
-    <mergeCell ref="A36:A37"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="A40:A41"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="A34:A35"/>
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="A24:A25"/>
     <mergeCell ref="A3:A4"/>
@@ -3224,6 +3213,18 @@
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="B13:B14"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="B32:B37"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="B40:B41"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="A40:A41"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.25" bottom="0.25" header="0" footer="0"/>

</xml_diff>